<commit_message>
removed non user-friendly prompts from femaleClients screenClient form.
</commit_message>
<xml_diff>
--- a/app/tables/femaleClients/forms/screenClient/screenClient.xlsx
+++ b/app/tables/femaleClients/forms/screenClient/screenClient.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31440" yWindow="1860" windowWidth="28800" windowHeight="16020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="31440" yWindow="1860" windowWidth="28800" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="217">
   <si>
     <t>type</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Enter months</t>
   </si>
   <si>
-    <t>Client is INELIGIBLE for the following reasons:</t>
-  </si>
-  <si>
     <t>Client is ELIGIBLE</t>
   </si>
   <si>
@@ -441,18 +438,6 @@
   </si>
   <si>
     <t>Thank you for considering being screened for the study. This will in no way affect the care that you, your children, or your partner will receive at the antenatal clinic.</t>
-  </si>
-  <si>
-    <t>- ${_ineligible_curr_relationship}</t>
-  </si>
-  <si>
-    <t>- ${_ineligible_partner_age}</t>
-  </si>
-  <si>
-    <t>- ${_ineligible_clinic_proximity}</t>
-  </si>
-  <si>
-    <t>If client is eligible for study, review previous questions and responses</t>
   </si>
   <si>
     <t>Thank you for your time in answering these questions. Based on some of the answers you gave, you are ineligible to be a part of the study. This in no way affects the care you will receive here at this clinic. Can I answer any questions you may have?</t>
@@ -563,18 +548,6 @@
   </si>
   <si>
     <t>test_result</t>
-  </si>
-  <si>
-    <t>ineligible_list</t>
-  </si>
-  <si>
-    <t>list_curr_rel</t>
-  </si>
-  <si>
-    <t>list_partner_age</t>
-  </si>
-  <si>
-    <t>list_clinic_prox</t>
   </si>
   <si>
     <t>ineligible_statement</t>
@@ -1316,7 +1289,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1362,9 +1335,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2269,25 +2239,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="13.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="24.5" style="19" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" style="21" customWidth="1"/>
     <col min="5" max="5" width="63" style="3" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" style="3" customWidth="1"/>
     <col min="7" max="8" width="10.83203125" style="3"/>
-    <col min="9" max="9" width="10.83203125" style="27"/>
+    <col min="9" max="9" width="10.83203125" style="26"/>
     <col min="10" max="10" width="10.83203125" style="3"/>
     <col min="11" max="11" width="15" style="3" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="3"/>
@@ -2297,22 +2267,22 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30">
       <c r="A1" s="3" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>2</v>
@@ -2320,7 +2290,7 @@
       <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -2352,116 +2322,116 @@
       <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="21" t="s">
-        <v>159</v>
+      <c r="C2" s="18"/>
+      <c r="D2" s="20" t="s">
+        <v>154</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>85</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="24"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:17" s="13" customFormat="1">
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="22" t="s">
-        <v>160</v>
+      <c r="C3" s="18"/>
+      <c r="D3" s="21" t="s">
+        <v>155</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:17" s="13" customFormat="1">
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="25"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:17" s="13" customFormat="1" ht="120">
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="22" t="s">
-        <v>161</v>
+      <c r="C5" s="18"/>
+      <c r="D5" s="21" t="s">
+        <v>156</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="I5" s="25"/>
+        <v>149</v>
+      </c>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1">
       <c r="B6" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C6" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>162</v>
+      <c r="D6" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="25" t="s">
-        <v>194</v>
+      <c r="I6" s="24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="13" customFormat="1" ht="45">
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="22" t="s">
-        <v>163</v>
+      <c r="C7" s="18"/>
+      <c r="D7" s="21" t="s">
+        <v>158</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="25"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:17" s="13" customFormat="1" ht="75">
       <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="22" t="s">
-        <v>164</v>
+      <c r="C8" s="18"/>
+      <c r="D8" s="21" t="s">
+        <v>159</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>194</v>
+        <v>151</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:17" s="13" customFormat="1" ht="45">
       <c r="B9" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>165</v>
+      <c r="D9" s="21" t="s">
+        <v>160</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>21</v>
@@ -2469,151 +2439,151 @@
       <c r="F9" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>194</v>
+      <c r="I9" s="24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:17" s="13" customFormat="1" ht="30">
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="22" t="s">
-        <v>166</v>
+      <c r="C10" s="18"/>
+      <c r="D10" s="21" t="s">
+        <v>161</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="24"/>
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:17" s="13" customFormat="1" ht="30">
       <c r="A11" s="13" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="22"/>
-      <c r="I11" s="25"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="21"/>
+      <c r="I11" s="24"/>
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:17" s="13" customFormat="1">
       <c r="B12" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>167</v>
+      <c r="D12" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="I12" s="25"/>
+      <c r="I12" s="24"/>
     </row>
     <row r="13" spans="1:17" s="13" customFormat="1">
       <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="22" t="s">
-        <v>168</v>
+      <c r="C13" s="18"/>
+      <c r="D13" s="21" t="s">
+        <v>163</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:17" s="13" customFormat="1">
       <c r="B14" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C14" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="22" t="s">
-        <v>169</v>
+      <c r="D14" s="21" t="s">
+        <v>164</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:17" s="13" customFormat="1">
       <c r="B15" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C15" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="26"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:17" s="13" customFormat="1">
       <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="22" t="s">
-        <v>170</v>
+      <c r="C16" s="18"/>
+      <c r="D16" s="21" t="s">
+        <v>165</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I16" s="25"/>
+      <c r="I16" s="24"/>
     </row>
     <row r="17" spans="1:9" s="13" customFormat="1" ht="30">
       <c r="B17" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="22" t="s">
-        <v>171</v>
+      <c r="D17" s="21" t="s">
+        <v>166</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="25"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9" s="13" customFormat="1">
       <c r="B18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="22" t="s">
-        <v>172</v>
+      <c r="C18" s="18"/>
+      <c r="D18" s="21" t="s">
+        <v>167</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="25"/>
+      <c r="I18" s="24"/>
     </row>
     <row r="19" spans="1:9" s="13" customFormat="1">
       <c r="A19" s="13" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="22"/>
-      <c r="I19" s="25"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="21"/>
+      <c r="I19" s="24"/>
     </row>
     <row r="20" spans="1:9" s="13" customFormat="1" ht="60">
       <c r="B20" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C20" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>173</v>
+      <c r="D20" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>55</v>
@@ -2621,17 +2591,17 @@
       <c r="F20" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I20" s="26" t="s">
-        <v>194</v>
+      <c r="I20" s="25" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="13" customFormat="1" ht="90">
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="22" t="s">
-        <v>174</v>
+      <c r="C21" s="18"/>
+      <c r="D21" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>73</v>
@@ -2640,45 +2610,45 @@
         <v>115</v>
       </c>
       <c r="H21" s="16"/>
-      <c r="I21" s="25" t="s">
-        <v>194</v>
+      <c r="I21" s="24" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="13" customFormat="1">
       <c r="B22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="22" t="s">
-        <v>175</v>
+      <c r="C22" s="18"/>
+      <c r="D22" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I22" s="26"/>
+      <c r="I22" s="25"/>
     </row>
     <row r="23" spans="1:9" s="13" customFormat="1">
       <c r="B23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="22" t="s">
-        <v>176</v>
+      <c r="C23" s="18"/>
+      <c r="D23" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I23" s="26"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" s="13" customFormat="1" ht="60">
       <c r="B24" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>177</v>
+      <c r="D24" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>47</v>
@@ -2686,236 +2656,181 @@
       <c r="F24" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="26" t="s">
-        <v>194</v>
+      <c r="I24" s="25" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="13" customFormat="1">
       <c r="B25" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="22" t="s">
-        <v>178</v>
+      <c r="D25" s="21" t="s">
+        <v>173</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="26"/>
+      <c r="I25" s="25"/>
     </row>
     <row r="26" spans="1:9" s="13" customFormat="1">
       <c r="B26" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C26" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="22" t="s">
-        <v>179</v>
+      <c r="D26" s="21" t="s">
+        <v>174</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="I26" s="26"/>
-    </row>
-    <row r="27" spans="1:9" s="13" customFormat="1" ht="45">
-      <c r="B27" s="8" t="s">
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:9" s="13" customFormat="1" ht="60">
+      <c r="B27" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="19"/>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="1:9" s="13" customFormat="1" ht="45">
+      <c r="B28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" s="13" customFormat="1" ht="60">
+      <c r="B29" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I29" s="24"/>
+    </row>
+    <row r="30" spans="1:9" s="13" customFormat="1" ht="45">
+      <c r="B30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="13" customFormat="1">
+      <c r="B31" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="13" customFormat="1" ht="30">
+      <c r="B32" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="I27" s="25"/>
-    </row>
-    <row r="28" spans="1:9" s="13" customFormat="1">
-      <c r="B28" s="8" t="s">
+      <c r="E32" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="2:9" s="13" customFormat="1">
+      <c r="B33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="2:9" s="13" customFormat="1" ht="60">
+      <c r="B34" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="I28" s="25"/>
-    </row>
-    <row r="29" spans="1:9" s="13" customFormat="1">
-      <c r="B29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="22" t="s">
+      <c r="C34" s="19"/>
+      <c r="D34" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="I29" s="25"/>
-    </row>
-    <row r="30" spans="1:9" s="13" customFormat="1">
-      <c r="B30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="I30" s="25"/>
-    </row>
-    <row r="31" spans="1:9" s="13" customFormat="1" ht="60">
-      <c r="B31" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="I31" s="25"/>
-    </row>
-    <row r="32" spans="1:9" s="13" customFormat="1" ht="45">
-      <c r="B32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="I32" s="25"/>
-    </row>
-    <row r="33" spans="2:9" s="13" customFormat="1" ht="60">
-      <c r="B33" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I33" s="25"/>
-    </row>
-    <row r="34" spans="2:9" s="13" customFormat="1" ht="45">
-      <c r="B34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="22" t="s">
-        <v>187</v>
-      </c>
       <c r="E34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>194</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I34" s="24"/>
     </row>
     <row r="35" spans="2:9" s="13" customFormat="1">
-      <c r="B35" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D35" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="I35" s="25" t="s">
-        <v>194</v>
-      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="21"/>
+      <c r="I35" s="24"/>
     </row>
     <row r="36" spans="2:9" s="13" customFormat="1" ht="30">
       <c r="B36" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>189</v>
+        <v>16</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I36" s="26"/>
-    </row>
-    <row r="37" spans="2:9" s="13" customFormat="1">
-      <c r="B37" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I37" s="26"/>
-    </row>
-    <row r="38" spans="2:9" s="13" customFormat="1" ht="60">
-      <c r="B38" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="I38" s="25"/>
-    </row>
-    <row r="39" spans="2:9" s="13" customFormat="1">
-      <c r="B39" s="8"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="22"/>
-      <c r="I39" s="25"/>
-    </row>
-    <row r="40" spans="2:9" s="13" customFormat="1" ht="30">
-      <c r="B40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="E40" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="I40" s="25"/>
+      <c r="I36" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2932,7 +2847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2946,13 +2861,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2960,7 +2875,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -2971,7 +2886,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>19</v>
@@ -2982,7 +2897,7 @@
         <v>121</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
@@ -2993,7 +2908,7 @@
         <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
@@ -3004,7 +2919,7 @@
         <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>86</v>
@@ -3015,7 +2930,7 @@
         <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>86</v>
@@ -3026,7 +2941,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -3037,7 +2952,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
@@ -3048,7 +2963,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
@@ -3059,7 +2974,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>26</v>
@@ -3070,7 +2985,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>27</v>
@@ -3081,7 +2996,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>28</v>
@@ -3092,7 +3007,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>69</v>
@@ -3103,7 +3018,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>86</v>
@@ -3114,7 +3029,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
@@ -3125,7 +3040,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
@@ -3136,7 +3051,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>33</v>
@@ -3147,7 +3062,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>34</v>
@@ -3158,7 +3073,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>35</v>
@@ -3169,7 +3084,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>36</v>
@@ -3180,7 +3095,7 @@
         <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>37</v>
@@ -3191,7 +3106,7 @@
         <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>38</v>
@@ -3202,7 +3117,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
@@ -3213,7 +3128,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>69</v>
@@ -3224,7 +3139,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>86</v>
@@ -3235,7 +3150,7 @@
         <v>130</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>87</v>
@@ -3246,7 +3161,7 @@
         <v>130</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>88</v>
@@ -3257,7 +3172,7 @@
         <v>130</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>45</v>
@@ -3268,7 +3183,7 @@
         <v>130</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>42</v>
@@ -3279,7 +3194,7 @@
         <v>130</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>43</v>
@@ -3290,7 +3205,7 @@
         <v>130</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>89</v>
@@ -3301,7 +3216,7 @@
         <v>130</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>44</v>
@@ -3312,7 +3227,7 @@
         <v>130</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>46</v>
@@ -3323,7 +3238,7 @@
         <v>130</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -3334,7 +3249,7 @@
         <v>130</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>69</v>
@@ -3345,7 +3260,7 @@
         <v>130</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>86</v>
@@ -3356,7 +3271,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>49</v>
@@ -3367,7 +3282,7 @@
         <v>48</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>50</v>
@@ -3378,7 +3293,7 @@
         <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>69</v>
@@ -3389,7 +3304,7 @@
         <v>48</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>86</v>
@@ -3400,7 +3315,7 @@
         <v>52</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
@@ -3411,7 +3326,7 @@
         <v>52</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>65</v>
@@ -3422,7 +3337,7 @@
         <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>86</v>
@@ -3433,7 +3348,7 @@
         <v>52</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>82</v>
@@ -3444,7 +3359,7 @@
         <v>97</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>18</v>
@@ -3455,7 +3370,7 @@
         <v>97</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>19</v>
@@ -3466,7 +3381,7 @@
         <v>97</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>86</v>
@@ -3477,7 +3392,7 @@
         <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>82</v>
@@ -3488,7 +3403,7 @@
         <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>90</v>
@@ -3499,7 +3414,7 @@
         <v>94</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>91</v>
@@ -3510,7 +3425,7 @@
         <v>94</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>92</v>
@@ -3521,7 +3436,7 @@
         <v>94</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>93</v>
@@ -3587,7 +3502,7 @@
         <v>74</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>75</v>
@@ -3598,7 +3513,7 @@
         <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>76</v>
@@ -3609,7 +3524,7 @@
         <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>77</v>
@@ -3620,7 +3535,7 @@
         <v>74</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>78</v>
@@ -3631,7 +3546,7 @@
         <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>79</v>
@@ -3642,7 +3557,7 @@
         <v>74</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>80</v>
@@ -3653,7 +3568,7 @@
         <v>74</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>86</v>
@@ -3664,7 +3579,7 @@
         <v>71</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>72</v>
@@ -3675,7 +3590,7 @@
         <v>99</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>100</v>
@@ -3686,7 +3601,7 @@
         <v>104</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>105</v>
@@ -3697,7 +3612,7 @@
         <v>104</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>106</v>
@@ -3708,7 +3623,7 @@
         <v>104</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>107</v>
@@ -3719,7 +3634,7 @@
         <v>104</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>108</v>
@@ -3730,7 +3645,7 @@
         <v>104</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>109</v>
@@ -3741,7 +3656,7 @@
         <v>104</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>110</v>
@@ -3752,7 +3667,7 @@
         <v>104</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>111</v>
@@ -3763,7 +3678,7 @@
         <v>104</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>112</v>
@@ -3774,7 +3689,7 @@
         <v>104</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>69</v>
@@ -3785,7 +3700,7 @@
         <v>104</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>86</v>
@@ -3796,7 +3711,7 @@
         <v>114</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>119</v>
@@ -3807,7 +3722,7 @@
         <v>131</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>133</v>
@@ -3818,7 +3733,7 @@
         <v>131</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>132</v>
@@ -3829,7 +3744,7 @@
         <v>131</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>86</v>
@@ -3840,10 +3755,10 @@
         <v>123</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -3851,7 +3766,7 @@
         <v>123</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>124</v>
@@ -3859,24 +3774,24 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3906,26 +3821,26 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B3" s="2">
         <v>20140512</v>
@@ -3933,18 +3848,18 @@
     </row>
     <row r="4" spans="1:3" ht="30">
       <c r="A4" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>